<commit_message>
Excel Utiliy added. LoginPageTest passed with values called from Excel sheet.
</commit_message>
<xml_diff>
--- a/7rmartSupermarketLiveProject/src/test/resources/7rmartSupermarketTestData.xlsx
+++ b/7rmartSupermarketLiveProject/src/test/resources/7rmartSupermarketTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrit\git\7rmartsupermarket\7rmartSupermarketLiveProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F7D42C7-3709-4B27-AA3B-468C35C04D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FF07BE-9E14-4A63-9F7B-A17EB33D79F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5028" yWindow="5148" windowWidth="17280" windowHeight="8880" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
+    <workbookView xWindow="5484" yWindow="2328" windowWidth="15708" windowHeight="8880" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -403,7 +404,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,4 +439,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67024343-FFBE-4F6E-86B2-AC28C9C7182F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Addeed all values in Excel utility
</commit_message>
<xml_diff>
--- a/7rmartSupermarketLiveProject/src/test/resources/7rmartSupermarketTestData.xlsx
+++ b/7rmartSupermarketLiveProject/src/test/resources/7rmartSupermarketTestData.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrit\git\7rmartsupermarket\7rmartSupermarketLiveProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FF07BE-9E14-4A63-9F7B-A17EB33D79F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC0834B-35F9-49D0-94CA-5BE7FD43C664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5484" yWindow="2328" windowWidth="15708" windowHeight="8880" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
+    <workbookView xWindow="11508" yWindow="6768" windowWidth="15708" windowHeight="8880" firstSheet="6" activeTab="7" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="ManageProductSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="ManageCategoryNew" sheetId="3" r:id="rId3"/>
+    <sheet name="ManageProductNew" sheetId="4" r:id="rId4"/>
+    <sheet name="ManageFooter" sheetId="5" r:id="rId5"/>
+    <sheet name="ManageContact" sheetId="6" r:id="rId6"/>
+    <sheet name="ManageNewsNew" sheetId="7" r:id="rId7"/>
+    <sheet name="AdminUsers" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>UserName</t>
   </si>
@@ -50,6 +56,81 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
+  </si>
+  <si>
+    <t>Curd12</t>
+  </si>
+  <si>
+    <t>P1015</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>P992</t>
+  </si>
+  <si>
+    <t>Category Value</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Title Value</t>
+  </si>
+  <si>
+    <t>max qty</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Asiatic business center,Technopark Phase three,Trivandrum</t>
+  </si>
+  <si>
+    <t>automationtesting@gmail.com</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>eMail</t>
+  </si>
+  <si>
+    <t>def@gmail.com</t>
+  </si>
+  <si>
+    <t>abc houseDiv 14, Kadavanthra, Panampilly Nagar,Ernakulam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Time </t>
+  </si>
+  <si>
+    <t>Delivery Charge Limit</t>
+  </si>
+  <si>
+    <t>Automation Today</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Obsqura2</t>
   </si>
 </sst>
 </file>
@@ -85,8 +166,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0199C51E-DBD8-4834-B9CB-972F535973D5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,12 +530,274 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67024343-FFBE-4F6E-86B2-AC28C9C7182F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33087168-0B8A-490A-8818-A6E05FC9FCE4}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A8251C-0835-4CC7-B11C-85A35805215D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213A25F4-AA7C-495E-BB23-D23351D4B1D1}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>9876543210</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926F525C-3D1B-4877-B7B1-1C9BC9C0896F}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA0E510-650A-42E5-9D74-2AD989FB0283}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0725FB86-5F8A-484B-933C-1B3E28394C09}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>214356</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated changes along with chaining
</commit_message>
<xml_diff>
--- a/7rmartSupermarketLiveProject/src/test/resources/7rmartSupermarketTestData.xlsx
+++ b/7rmartSupermarketLiveProject/src/test/resources/7rmartSupermarketTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrit\git\7rmartsupermarket\7rmartSupermarketLiveProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2328C6E3-F337-4893-9FFF-0894A3A83770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF36A93-BC68-48A9-A821-8D9EB1E98BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="3708" windowWidth="15708" windowHeight="8880" firstSheet="6" activeTab="7" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
+    <workbookView xWindow="5160" yWindow="3360" windowWidth="15708" windowHeight="8880" activeTab="1" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>UserName</t>
   </si>
@@ -64,12 +64,6 @@
     <t>ProductCode</t>
   </si>
   <si>
-    <t>Curd12</t>
-  </si>
-  <si>
-    <t>P1015</t>
-  </si>
-  <si>
     <t>Milk</t>
   </si>
   <si>
@@ -130,20 +124,35 @@
     <t>News</t>
   </si>
   <si>
-    <t>Obsqura2</t>
+    <t>Amritha</t>
+  </si>
+  <si>
+    <t>ammu</t>
+  </si>
+  <si>
+    <t>Mutton</t>
+  </si>
+  <si>
+    <t>Nonveg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -174,6 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67024343-FFBE-4F6E-86B2-AC28C9C7182F}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -549,24 +559,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -575,7 +586,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,12 +596,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -614,21 +625,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>45</v>
@@ -649,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213A25F4-AA7C-495E-BB23-D23351D4B1D1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -662,21 +673,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>9876543210</v>
@@ -706,19 +717,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -726,10 +737,10 @@
         <v>2255</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -758,12 +769,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -775,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0725FB86-5F8A-484B-933C-1B3E28394C09}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,10 +805,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2">
-        <v>214356</v>
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>